<commit_message>
só dando update msm :)
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -1433,6 +1433,24 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
+      <c r="T17" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="U17" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="W17" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="X17" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3">

</xml_diff>